<commit_message>
finished till select 2 companies
Have added all the companies and their bios + prices in a seperate package.

Ready for creating scenarios and market manipulation.
</commit_message>
<xml_diff>
--- a/Planning/Planning & To-Do.xlsx
+++ b/Planning/Planning & To-Do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de73362643db60d3/Documents/GitHub/SimulatedStockMarket/Planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobby\OneDrive\Documents\SimulatedStockMarket\SimulatedStockMarket\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC10486479DB79E65BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C5B29C3-4DD9-487C-B119-84A78BE56FD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF9AD55-9703-46C0-80E1-8F2E51FB7040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TO-DO</t>
   </si>
@@ -39,7 +39,16 @@
     <t>Welcome / Sign up</t>
   </si>
   <si>
-    <t>Login</t>
+    <t xml:space="preserve">Up &amp; coming Start-Up Companies w/ descriptions  </t>
+  </si>
+  <si>
+    <t>Daily news reports</t>
+  </si>
+  <si>
+    <t>10 days</t>
+  </si>
+  <si>
+    <t>random array of companies</t>
   </si>
 </sst>
 </file>
@@ -393,21 +402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G7"/>
+  <dimension ref="C3:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="31.77734375" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="3:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,14 +427,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>